<commit_message>
Added index name in processed results
</commit_message>
<xml_diff>
--- a/test_results/06_03_137.xlsx
+++ b/test_results/06_03_137.xlsx
@@ -255,7 +255,7 @@
     <t>End (Test)</t>
   </si>
   <si>
-    <t>01:00</t>
+    <t>00:30</t>
   </si>
   <si>
     <t>Duration</t>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -449,7 +449,10 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4655,7 +4658,7 @@
       <c r="E8" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4675,8 +4678,8 @@
       <c r="E9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="15">
-        <v>60.0</v>
+      <c r="F9" s="16">
+        <v>30.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>